<commit_message>
Use 105 PPFD to match 30 minute twilight in Twilight length alters growth and flowering time in Arabidopsis via LHY/CCA1
</commit_message>
<xml_diff>
--- a/experiments/online/E10/P0/balanced.xlsx
+++ b/experiments/online/E10/P0/balanced.xlsx
@@ -151,28 +151,11 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -182,6 +165,15 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="10"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -203,7 +195,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -237,14 +229,11 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
@@ -278,8 +267,8 @@
       <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffb5cea8"/>
-      <rgbColor rgb="ff1e1e1e"/>
+      <rgbColor rgb="cc99cccc"/>
+      <rgbColor rgb="ff2a2d2e"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -417,13 +406,7 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
+          <a:effectLst/>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -521,10 +504,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -770,13 +753,7 @@
           <a:prstDash val="solid"/>
           <a:round/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
+        <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
@@ -1078,10 +1055,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Cambria"/>
-            <a:ea typeface="Cambria"/>
-            <a:cs typeface="Cambria"/>
-            <a:sym typeface="Cambria"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1369,7 +1346,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5">
-        <v>1.374988425925926</v>
+        <v>2.374988425925926</v>
       </c>
       <c r="C2" s="6">
         <v>0</v>
@@ -1398,27 +1375,27 @@
         <v>0</v>
       </c>
       <c r="B3" s="9">
-        <v>1.375</v>
+        <v>2.375</v>
       </c>
       <c r="C3" s="10">
-        <v>22.5</v>
-      </c>
-      <c r="D3" s="11">
-        <v>81</v>
-      </c>
-      <c r="E3" s="11">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>7.2</v>
-      </c>
-      <c r="H3" s="12">
-        <v>14.2</v>
-      </c>
-      <c r="I3" s="13">
+        <v>19.6875</v>
+      </c>
+      <c r="D3" s="10">
+        <v>70.875</v>
+      </c>
+      <c r="E3" s="10">
+        <v>8.137499999999999</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>6.3</v>
+      </c>
+      <c r="H3" s="10">
+        <v>12.425</v>
+      </c>
+      <c r="I3" s="11">
         <v>1</v>
       </c>
     </row>
@@ -1427,36 +1404,36 @@
         <v>0</v>
       </c>
       <c r="B4" s="9">
-        <v>1.875</v>
-      </c>
-      <c r="C4" s="10">
-        <v>22.5</v>
-      </c>
-      <c r="D4" s="11">
-        <v>81</v>
-      </c>
-      <c r="E4" s="11">
-        <v>9.300000000000001</v>
-      </c>
-      <c r="F4" s="11">
-        <v>0</v>
-      </c>
-      <c r="G4" s="11">
-        <v>7.2</v>
+        <v>2.875</v>
+      </c>
+      <c r="C4" s="12">
+        <v>19.6875</v>
+      </c>
+      <c r="D4" s="12">
+        <v>70.875</v>
+      </c>
+      <c r="E4" s="12">
+        <v>8.137499999999999</v>
+      </c>
+      <c r="F4" s="12">
+        <v>0</v>
+      </c>
+      <c r="G4" s="12">
+        <v>6.3</v>
       </c>
       <c r="H4" s="12">
-        <v>14.2</v>
-      </c>
-      <c r="I4" s="13">
+        <v>12.425</v>
+      </c>
+      <c r="I4" s="11">
         <v>1</v>
       </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" s="14">
-        <v>0</v>
-      </c>
-      <c r="B5" s="15">
-        <v>1.875011574074074</v>
+      <c r="A5" s="13">
+        <v>0</v>
+      </c>
+      <c r="B5" s="14">
+        <v>2.875011574074074</v>
       </c>
       <c r="C5" s="6">
         <v>0</v>
@@ -1476,64 +1453,64 @@
       <c r="H5" s="6">
         <v>0</v>
       </c>
-      <c r="I5" s="16">
+      <c r="I5" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" s="17"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
     </row>
     <row r="7" ht="13.55" customHeight="1">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
+      <c r="A7" s="16"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
     </row>
     <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
     </row>
     <row r="9" ht="13.55" customHeight="1">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
     </row>
     <row r="10" ht="13.55" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="17"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
+      <c r="A10" s="16"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511806" footer="0.511806"/>

</xml_diff>